<commit_message>
feat: add PIE and USPS_MNIST dataset
</commit_message>
<xml_diff>
--- a/results/mk-mmcd.xlsx
+++ b/results/mk-mmcd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caokang/Documents/MEDA/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1CD321-70FC-1242-841E-278667B1BC98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5247C8B8-1DDE-8B4D-AA88-924B167AD661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{21FD61EE-2419-D345-9765-2E447AB1C80B}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{21FD61EE-2419-D345-9765-2E447AB1C80B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>MEDA</t>
   </si>
@@ -88,6 +88,78 @@
   </si>
   <si>
     <t>D-&gt;W</t>
+  </si>
+  <si>
+    <t>USOS_MNIST</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>relative performance</t>
+  </si>
+  <si>
+    <t>PIE</t>
+  </si>
+  <si>
+    <t>05-&gt;07</t>
+  </si>
+  <si>
+    <t>05-&gt;09</t>
+  </si>
+  <si>
+    <t>05-&gt;27</t>
+  </si>
+  <si>
+    <t>05-&gt;29</t>
+  </si>
+  <si>
+    <t>07-&gt;05</t>
+  </si>
+  <si>
+    <t>07-&gt;09</t>
+  </si>
+  <si>
+    <t>07-&gt;27</t>
+  </si>
+  <si>
+    <t>07-&gt;29</t>
+  </si>
+  <si>
+    <t>09-&gt;05</t>
+  </si>
+  <si>
+    <t>09-&gt;07</t>
+  </si>
+  <si>
+    <t>09-&gt;27</t>
+  </si>
+  <si>
+    <t>09-&gt;29</t>
+  </si>
+  <si>
+    <t>27-&gt;05</t>
+  </si>
+  <si>
+    <t>27-&gt;07</t>
+  </si>
+  <si>
+    <t>27-&gt;09</t>
+  </si>
+  <si>
+    <t>27-&gt;29</t>
+  </si>
+  <si>
+    <t>29-&gt;05</t>
+  </si>
+  <si>
+    <t>29-&gt;07</t>
+  </si>
+  <si>
+    <t>29-&gt;09</t>
+  </si>
+  <si>
+    <t>29-&gt;27</t>
   </si>
 </sst>
 </file>
@@ -97,7 +169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,6 +179,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,11 +223,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DD1D7E-C6DB-B14F-BED2-9726A1A9321D}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1253,7 +1333,7 @@
         <v>4.0677966101695051E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1263,7 +1343,7 @@
         <v>3.1847133757960999E-2</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1">
         <f t="shared" si="2"/>
         <v>-1.7809439002670069E-3</v>
@@ -1273,7 +1353,7 @@
         <v>2.6714158504009822E-3</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1283,7 +1363,7 @@
         <v>3.1315240083510387E-3</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="1">
         <f t="shared" si="2"/>
         <v>6.3694267515919112E-3</v>
@@ -1293,7 +1373,7 @@
         <v>-2.5477707006368977E-2</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="1">
         <f t="shared" si="2"/>
         <v>8.9047195013397529E-4</v>
@@ -1303,7 +1383,7 @@
         <v>8.0142475512020028E-3</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="1">
         <f t="shared" si="2"/>
         <v>5.2192066805839543E-3</v>
@@ -1313,7 +1393,7 @@
         <v>1.0438413361170129E-3</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1323,10 +1403,229 @@
         <v>-1.3559322033898979E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C57" s="1">
         <f>SUM(C44:C55)/12</f>
         <v>1.4350769905895183E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B60" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0.88722222222222202</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B61" s="1">
+        <v>0.748</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0.73550000000000004</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B64" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64" s="1">
+        <f>C60-$B60</f>
+        <v>-2.77777777777799E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="1">
+        <f>C61-$B61</f>
+        <v>-1.2499999999999956E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" s="1">
+        <f>AVERAGE(C64:C65)</f>
+        <v>-7.6388888888889728E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0.39472068753836698</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0.44607843137254899</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.64854310603784904</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0.340073529411765</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.46278511404561801</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0.50796568627451</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.71312706518474001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0.46878751500600202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0.488029465930018</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0.72874737158305802</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0.45465686274509798</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B83" s="1">
+        <v>0.70048019207683099</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0.74708410067526099</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.82046568627451</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.54901960784313697</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.38955582232893199</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.37323511356660499</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0.44546568627451</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.53259237008110505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: correct mmcd computation
</commit_message>
<xml_diff>
--- a/results/mk-mmcd.xlsx
+++ b/results/mk-mmcd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caokang/Documents/MEDA/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5247C8B8-1DDE-8B4D-AA88-924B167AD661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92452EB-1AB1-EE45-902A-8EFF4A01591A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{21FD61EE-2419-D345-9765-2E447AB1C80B}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16240" xr2:uid="{21FD61EE-2419-D345-9765-2E447AB1C80B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>MEDA</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>29-&gt;27</t>
+  </si>
+  <si>
+    <t>COIL</t>
+  </si>
+  <si>
+    <t>COIL_01</t>
+  </si>
+  <si>
+    <t>COIL_02</t>
+  </si>
+  <si>
+    <t>平均</t>
   </si>
 </sst>
 </file>
@@ -543,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DD1D7E-C6DB-B14F-BED2-9726A1A9321D}">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,7 +571,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,7 +591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -601,8 +613,11 @@
       <c r="G2" s="1">
         <v>0.56889352818371597</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>0.56471816283924903</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -624,8 +639,11 @@
       <c r="G3" s="1">
         <v>0.58305084745762703</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <v>0.54237288135593198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -647,8 +665,11 @@
       <c r="G4" s="1">
         <v>0.58598726114649702</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="1">
+        <v>0.50318471337579596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -670,8 +691,11 @@
       <c r="G5" s="1">
         <v>0.43989314336598401</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <v>0.446126447016919</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -693,8 +717,11 @@
       <c r="G6" s="1">
         <v>0.471186440677966</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="1">
+        <v>0.54915254237288103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -716,8 +743,11 @@
       <c r="G7" s="1">
         <v>0.452229299363057</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="1">
+        <v>0.45859872611465002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -739,8 +769,11 @@
       <c r="G8" s="1">
         <v>0.35351736420302798</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="1">
+        <v>0.33748886910062298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -762,8 +795,11 @@
       <c r="G9" s="1">
         <v>0.419624217118998</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="1">
+        <v>0.42901878914405001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -785,8 +821,11 @@
       <c r="G10" s="1">
         <v>0.78343949044586003</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="1">
+        <v>0.88535031847133805</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -808,8 +847,11 @@
       <c r="G11" s="1">
         <v>0.365093499554764</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="1">
+        <v>0.34995547640249303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -831,8 +873,11 @@
       <c r="G12" s="1">
         <v>0.40814196242171202</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="1">
+        <v>0.41544885177453</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -854,13 +899,16 @@
       <c r="G13" s="1">
         <v>0.827118644067797</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="1">
+        <v>0.87457627118644099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:G26" si="0">C2-$B2</f>
+        <f t="shared" ref="C15:I26" si="0">C2-$B2</f>
         <v>1.0438413361170129E-3</v>
       </c>
       <c r="D15" s="1">
@@ -879,8 +927,12 @@
         <f t="shared" si="0"/>
         <v>3.1315240083509277E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.0438413361160137E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -904,8 +956,12 @@
         <f t="shared" si="0"/>
         <v>4.4067796610169019E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H16" s="1">
+        <f t="shared" ref="H16:I16" si="1">H3-$B3</f>
+        <v>3.3898305084739677E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -929,8 +985,12 @@
         <f t="shared" si="0"/>
         <v>8.2802547770701063E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H17" s="1">
+        <f t="shared" ref="H17:I17" si="2">H4-$B4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
@@ -954,8 +1014,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="1">
+        <f t="shared" ref="H18:I18" si="3">H5-$B5</f>
+        <v>6.2333036509349959E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -979,8 +1043,12 @@
         <f t="shared" si="0"/>
         <v>-6.1016949152542965E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="1">
+        <f t="shared" ref="H19:I19" si="4">H6-$B6</f>
+        <v>1.6949152542372059E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
@@ -1004,8 +1072,12 @@
         <f t="shared" si="0"/>
         <v>-6.3694267515930214E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="1">
+        <f t="shared" ref="H20:I20" si="5">H7-$B7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -1029,8 +1101,12 @@
         <f t="shared" si="0"/>
         <v>1.157613535173696E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="1">
+        <f t="shared" ref="H21:I21" si="6">H8-$B8</f>
+        <v>-4.4523597506680446E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -1054,8 +1130,12 @@
         <f t="shared" si="0"/>
         <v>-7.3068893528179801E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="1">
+        <f t="shared" ref="H22:I22" si="7">H9-$B9</f>
+        <v>2.0876826722340258E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -1079,8 +1159,12 @@
         <f t="shared" si="0"/>
         <v>-0.10191082802547802</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="1">
+        <f t="shared" ref="H23:I23" si="8">H10-$B10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
@@ -1104,8 +1188,12 @@
         <f t="shared" si="0"/>
         <v>1.6918967052537981E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="1">
+        <f t="shared" ref="H24:I24" si="9">H11-$B11</f>
+        <v>1.7809439002670069E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -1129,8 +1217,12 @@
         <f t="shared" si="0"/>
         <v>-4.1753653444679961E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H25" s="1">
+        <f t="shared" ref="H25:I25" si="10">H12-$B12</f>
+        <v>3.131524008349984E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>18</v>
       </c>
@@ -1154,40 +1246,48 @@
         <f t="shared" si="0"/>
         <v>-4.7457627118643986E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="1">
+        <f t="shared" ref="H26:I26" si="11">H13-$B13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C28" s="1">
-        <f>SUM(C15:C26)/12</f>
+        <f t="shared" ref="C28:I28" si="12">SUM(C15:C26)/12</f>
         <v>8.8006433334015723E-3</v>
       </c>
       <c r="D28" s="1">
-        <f>SUM(D15:D26)/12</f>
+        <f t="shared" si="12"/>
         <v>1.2665927802382237E-2</v>
       </c>
       <c r="E28" s="1">
-        <f>SUM(E15:E26)/12</f>
+        <f t="shared" si="12"/>
         <v>2.5895433620868277E-3</v>
       </c>
       <c r="F28" s="1">
-        <f>SUM(F15:F26)/12</f>
+        <f t="shared" si="12"/>
         <v>9.1805946906799076E-3</v>
       </c>
       <c r="G28" s="1">
-        <f>SUM(G15:G26)/12</f>
+        <f t="shared" si="12"/>
         <v>-5.811676246004001E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="1">
+        <f t="shared" si="12"/>
+        <v>2.3396863496539986E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
         <v>0.56680584551148205</v>
       </c>
@@ -1195,7 +1295,7 @@
         <v>0.56471816283924903</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
         <v>0.53898305084745801</v>
       </c>
@@ -1289,117 +1389,117 @@
         <v>1.0438413361170129E-3</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" ref="C44:C55" si="1">C31-$B31</f>
+        <f t="shared" ref="C44:C55" si="13">C31-$B31</f>
         <v>-2.0876826722330266E-3</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" s="1">
-        <f t="shared" ref="B45:B55" si="2">B32-B3</f>
+        <f t="shared" ref="B45:B55" si="14">B32-B3</f>
         <v>0</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.0338983050847026E-2</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>0.10828025477707004</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>6.2333036509349959E-3</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>-2.6714158504009822E-3</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>1.0169491525423013E-2</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>4.0677966101695051E-2</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>3.1847133757960999E-2</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>-1.7809439002670069E-3</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>2.6714158504009822E-3</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>3.1315240083510387E-3</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>6.3694267515919112E-3</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>-2.5477707006368977E-2</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>8.9047195013397529E-4</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>8.0142475512020028E-3</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>5.2192066805839543E-3</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>1.0438413361170129E-3</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>-1.3559322033898979E-2</v>
       </c>
     </row>
@@ -1427,6 +1527,9 @@
       <c r="C60" s="1">
         <v>0.88722222222222202</v>
       </c>
+      <c r="D60" s="1">
+        <v>0.72222222222222199</v>
+      </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="1">
@@ -1435,6 +1538,9 @@
       <c r="C61" s="1">
         <v>0.73550000000000004</v>
       </c>
+      <c r="D61" s="1">
+        <v>0.62549999999999994</v>
+      </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
@@ -1444,14 +1550,22 @@
         <f>C60-$B60</f>
         <v>-2.77777777777799E-3</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" s="1">
+        <f>D60-$B60</f>
+        <v>-0.16777777777777803</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C65" s="1">
         <f>C61-$B61</f>
         <v>-1.2499999999999956E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" s="1">
+        <f>D61-$B61</f>
+        <v>-0.12250000000000005</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>20</v>
       </c>
@@ -1460,7 +1574,7 @@
         <v>-7.6388888888889728E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>22</v>
       </c>
@@ -1468,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>23</v>
       </c>
@@ -1476,7 +1590,7 @@
         <v>0.39472068753836698</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>24</v>
       </c>
@@ -1484,7 +1598,7 @@
         <v>0.44607843137254899</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>25</v>
       </c>
@@ -1492,7 +1606,7 @@
         <v>0.64854310603784904</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>26</v>
       </c>
@@ -1500,7 +1614,7 @@
         <v>0.340073529411765</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>27</v>
       </c>
@@ -1508,7 +1622,7 @@
         <v>0.46278511404561801</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>28</v>
       </c>
@@ -1516,7 +1630,7 @@
         <v>0.50796568627451</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>29</v>
       </c>
@@ -1524,7 +1638,7 @@
         <v>0.71312706518474001</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>30</v>
       </c>
@@ -1532,7 +1646,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>31</v>
       </c>
@@ -1540,7 +1654,7 @@
         <v>0.46878751500600202</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>32</v>
       </c>
@@ -1548,7 +1662,7 @@
         <v>0.488029465930018</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>33</v>
       </c>
@@ -1556,7 +1670,7 @@
         <v>0.72874737158305802</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>34</v>
       </c>
@@ -1564,7 +1678,7 @@
         <v>0.45465686274509798</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>35</v>
       </c>
@@ -1572,7 +1686,7 @@
         <v>0.70048019207683099</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>36</v>
       </c>
@@ -1580,7 +1694,7 @@
         <v>0.74708410067526099</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>37</v>
       </c>
@@ -1588,7 +1702,7 @@
         <v>0.82046568627451</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>38</v>
       </c>
@@ -1596,7 +1710,7 @@
         <v>0.54901960784313697</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>39</v>
       </c>
@@ -1604,7 +1718,7 @@
         <v>0.38955582232893199</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>40</v>
       </c>
@@ -1612,7 +1726,7 @@
         <v>0.37323511356660499</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>41</v>
       </c>
@@ -1620,12 +1734,143 @@
         <v>0.44546568627451</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B90" s="1">
         <v>0.53259237008110505</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0.90138888888888902</v>
+      </c>
+      <c r="C93" s="1">
+        <v>0.86805555555555602</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0.88472222222222197</v>
+      </c>
+      <c r="E93" s="1">
+        <v>0.88888888888888895</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0.89861111111111103</v>
+      </c>
+      <c r="G93" s="1">
+        <v>0.86388888888888904</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0.87083333333333302</v>
+      </c>
+      <c r="C94" s="1">
+        <v>0.85972222222222205</v>
+      </c>
+      <c r="D94" s="1">
+        <v>0.87083333333333302</v>
+      </c>
+      <c r="E94" s="1">
+        <v>0.87083333333333302</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0.87083333333333302</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0.85416666666666696</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C96" s="1">
+        <f>C93-$B93</f>
+        <v>-3.3333333333332993E-2</v>
+      </c>
+      <c r="D96" s="1">
+        <f>D93-$B93</f>
+        <v>-1.6666666666667052E-2</v>
+      </c>
+      <c r="E96" s="1">
+        <f>E93-$B93</f>
+        <v>-1.2500000000000067E-2</v>
+      </c>
+      <c r="F96" s="1">
+        <f>F93-$B93</f>
+        <v>-2.77777777777799E-3</v>
+      </c>
+      <c r="G96" s="1">
+        <f>G93-$B93</f>
+        <v>-3.7499999999999978E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C97" s="1">
+        <f>C94-B94</f>
+        <v>-1.1111111111110961E-2</v>
+      </c>
+      <c r="D97" s="1">
+        <f>D94-$B94</f>
+        <v>0</v>
+      </c>
+      <c r="E97" s="1">
+        <f>E94-$B94</f>
+        <v>0</v>
+      </c>
+      <c r="F97" s="1">
+        <f>F94-$B94</f>
+        <v>0</v>
+      </c>
+      <c r="G97" s="1">
+        <f>G94-$B94</f>
+        <v>-1.6666666666666052E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B98" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C99" s="1">
+        <f>AVERAGE(C96:C97)</f>
+        <v>-2.2222222222221977E-2</v>
+      </c>
+      <c r="D99" s="1">
+        <f t="shared" ref="D99:G99" si="15">AVERAGE(D96:D97)</f>
+        <v>-8.3333333333335258E-3</v>
+      </c>
+      <c r="E99" s="1">
+        <f t="shared" si="15"/>
+        <v>-6.2500000000000333E-3</v>
+      </c>
+      <c r="F99" s="1">
+        <f t="shared" si="15"/>
+        <v>-1.388888888888995E-3</v>
+      </c>
+      <c r="G99" s="1">
+        <f t="shared" si="15"/>
+        <v>-2.7083333333333015E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>